<commit_message>
perubahan pada tampilan peta dan web
</commit_message>
<xml_diff>
--- a/public/Data-Toko-Contoh-import.xlsx
+++ b/public/Data-Toko-Contoh-import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\webgis-toko\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E2B839-602E-4C97-AA35-AEEEEF4D17E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E398E5-F07A-49A8-8E6C-C9C95519820B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,15 +19,223 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>ASUS TUF</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{7A15E2A1-6BC8-4D91-AD1B-010B9B9FA497}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tidak Wajib diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{0CFA129C-5B6D-42A8-8D9D-B46D23AE9782}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wajib Diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{31C55B3A-2FD3-4F12-AE21-302B30D6A843}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wajib Diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{E237B5D7-E091-4D4A-AEB9-24DF32D83E30}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wajib Diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{E45AFC80-1C6E-4155-8B7F-576829C6C085}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wajib Diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{F3CDF675-757F-4BF9-AA1E-6F50FC326608}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tidak Wajib Diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{BD82A7B2-1A2C-416F-91A6-EA6AB632F946}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wajib Diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{BCE95709-5AEF-4781-BD93-50098B7A9EB6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wajib Diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{94EF8673-7621-432A-8478-4BB8313C6695}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wajib Diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{12DB7F55-25E9-4B87-A9D1-F95D6C632747}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wajib Diisi
+Memasukkan Kecamatan Dari Lokasi Toko</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{55746554-8E7E-4730-8E8C-01055F3F10C0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wajib Diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{69C6E993-FE6B-47B3-8C0D-1567ABB591D0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wajib Diisi
+Pilih Jenis Usaha Berdasarkan Omset Usaha:
+Usaha Mikro (Maksimal Rp 300 juta)
+Usaha Kecil (Lebih dari Rp 300 juta – Rp 2,5 miliar)
+Usaha Menengah (Lebih dari Rp 2,5 miliar – Rp 50 miliar)
+Usaha Besar (Lebih dari Rp 50 miliar)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{14E943A7-ABD8-4D7A-8D19-C42E70AB5262}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wajib Diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{FE8A2F2D-F4F9-4B75-A876-51FA2623240D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wajib Diisi</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Nomo NIB</t>
-  </si>
-  <si>
     <t>Nomor KTP</t>
   </si>
   <si>
@@ -70,46 +278,85 @@
     <t>Tanjung Redeb</t>
   </si>
   <si>
-    <t>Toko Berkat Abadi</t>
-  </si>
-  <si>
-    <t>Jl. Kapten Tendean, Bugis, Kec. Tj. Redeb, Kabupaten Berau, Kalimantan Timur 77352</t>
-  </si>
-  <si>
-    <t>Toko Nuur Azizah</t>
-  </si>
-  <si>
-    <t>Jl. AKB Sanipah 1, Karang Ambun, Kec. Tj. Redeb, Kabupaten Berau, Kalimantan Timur 77315</t>
-  </si>
-  <si>
-    <t>Toko Hj. Aminah</t>
-  </si>
-  <si>
-    <t>Jl. H. Isa II, Karang Ambun, Kec. Tj. Redeb, Kabupaten Berau, Kalimantan Timur 77315</t>
-  </si>
-  <si>
-    <t>Warung Sudirman</t>
-  </si>
-  <si>
-    <t>Jl. Mangga III, Karang Ambun, Kec. Tj. Redeb, Kabupaten Berau, Kalimantan Timur 77315</t>
-  </si>
-  <si>
-    <t>hamdi2003</t>
-  </si>
-  <si>
-    <t>holysword012</t>
-  </si>
-  <si>
-    <t>hamdilamela@gmail.com</t>
-  </si>
-  <si>
-    <t>081211098381</t>
-  </si>
-  <si>
     <t>Sembako</t>
   </si>
   <si>
-    <t>Usaha Kecil</t>
+    <t>example1</t>
+  </si>
+  <si>
+    <t>example2</t>
+  </si>
+  <si>
+    <t>example3</t>
+  </si>
+  <si>
+    <t>example1@gmail.com</t>
+  </si>
+  <si>
+    <t>example2@gmail.com</t>
+  </si>
+  <si>
+    <t>example3@gmail.com</t>
+  </si>
+  <si>
+    <t>081239481723</t>
+  </si>
+  <si>
+    <t>081239481724</t>
+  </si>
+  <si>
+    <t>081239481725</t>
+  </si>
+  <si>
+    <t>Usaha Mikro</t>
+  </si>
+  <si>
+    <t>9282270801212070</t>
+  </si>
+  <si>
+    <t>7728134781356241</t>
+  </si>
+  <si>
+    <t>6573252313213089</t>
+  </si>
+  <si>
+    <t>0475702763326330</t>
+  </si>
+  <si>
+    <t>6074058145695553</t>
+  </si>
+  <si>
+    <t>0428893647145315</t>
+  </si>
+  <si>
+    <t>4946575936762327</t>
+  </si>
+  <si>
+    <t>3676212210363274</t>
+  </si>
+  <si>
+    <t>7250864528092341</t>
+  </si>
+  <si>
+    <t>Toko Example1</t>
+  </si>
+  <si>
+    <t>Toko Example3</t>
+  </si>
+  <si>
+    <t>Toko Example2</t>
+  </si>
+  <si>
+    <t>Jalan Example1</t>
+  </si>
+  <si>
+    <t>Jalan Example2</t>
+  </si>
+  <si>
+    <t>Jalan Example3</t>
+  </si>
+  <si>
+    <t>Nomor NIB</t>
   </si>
 </sst>
 </file>
@@ -119,7 +366,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -145,6 +392,30 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -160,27 +431,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -203,14 +459,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -220,15 +475,23 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -533,11 +796,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,190 +824,201 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="L2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="10">
+        <v>2.1605932506428198</v>
+      </c>
+      <c r="O2" s="10">
+        <v>117.498464434512</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1203849172634560</v>
-      </c>
-      <c r="C2" s="3">
-        <v>293816475839261</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1029384675384950</v>
-      </c>
-      <c r="E2" s="5" t="s">
+    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="10">
+        <v>2.1551592749166599</v>
+      </c>
+      <c r="O3" s="10">
+        <v>117.501822446454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="I4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="8">
-        <v>2.1605932506428198</v>
-      </c>
-      <c r="O2" s="8">
-        <v>117.498464434512</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="8">
-        <v>2.1551592749166599</v>
-      </c>
-      <c r="O3" s="8">
-        <v>117.501822446454</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="8">
+      <c r="N4" s="10">
         <v>2.14956534126532</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="10">
         <v>117.500003183072</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="8">
-        <v>2.1448050960929099</v>
-      </c>
-      <c r="O5" s="8">
-        <v>117.505207873469</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{C6C97A93-FAAB-40E1-997F-9809B4B4C508}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{B4C387A0-2FC1-4B8E-B2C9-5D2CC7C60865}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{35F513FE-1F06-4513-8B88-D14B51B153C9}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{B032FDCF-2FD6-4490-9529-F4BDB6BD719B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>